<commit_message>
Need to implement for real the message passing. Have general structure
</commit_message>
<xml_diff>
--- a/Message Passing.xlsx
+++ b/Message Passing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\PGM Continued\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302F325D-6D4E-450B-8E44-C3DF77DBA9C5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBC7A2F-0F32-4D8D-B7FE-DADAB7A054A1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12225" tabRatio="333" xr2:uid="{B01DCFA4-244F-4B40-81FA-3205ACC7EABC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t xml:space="preserve">Approach 1 </t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Have a Node Dictionary</t>
+  </si>
+  <si>
+    <t>map to message</t>
   </si>
 </sst>
 </file>
@@ -464,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28252AC2-57BA-441C-98E4-C804E26D626D}">
-  <dimension ref="A3:I20"/>
+  <dimension ref="A3:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -481,7 +484,7 @@
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
@@ -494,7 +497,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
@@ -509,7 +512,7 @@
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -534,7 +537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -551,7 +554,7 @@
       </c>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -570,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -587,12 +590,12 @@
       </c>
       <c r="I8" s="3"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -600,27 +603,30 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>10</v>
       </c>

</xml_diff>